<commit_message>
Imagen a juegos en dino
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 1ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 1ª Version.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hahdm\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hahdm\Workspace\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE58898-F407-47BA-B33F-978717478EFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CD8706-E169-4F8F-93E0-E9CB845FE7EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -899,7 +899,7 @@
   <dimension ref="A2:P61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -953,7 +953,7 @@
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>135.69999999999999</v>
+        <v>137.19999999999999</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="4" t="s">
@@ -961,7 +961,7 @@
       </c>
       <c r="K3" s="2">
         <f>F6+F12+F22+F21+F52+F53+F54</f>
-        <v>36</v>
+        <v>37.5</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1301,7 +1301,7 @@
         <v>3</v>
       </c>
       <c r="F21" s="1">
-        <v>23.5</v>
+        <v>24</v>
       </c>
       <c r="G21" s="7"/>
     </row>
@@ -1825,7 +1825,9 @@
       <c r="E53" s="1">
         <v>1</v>
       </c>
-      <c r="F53" s="1"/>
+      <c r="F53" s="1">
+        <v>1</v>
+      </c>
       <c r="G53" s="1" t="s">
         <v>47</v>
       </c>
@@ -2043,7 +2045,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>2</v>
       </c>
@@ -2064,7 +2066,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -2250,7 +2252,7 @@
       </c>
       <c r="G17" s="11"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A18" s="13">
         <v>17</v>
       </c>
@@ -2271,7 +2273,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A19" s="13">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Actualizacion excel y eliminacion de carga.js
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 1ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 1ª Version.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hahdm\Workspace\Konguitos_Casino\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611E377B-F65C-4A86-8031-8D5E22E4F905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4834D3D7-9853-43AF-AC63-D2F1F0DD893A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificador" sheetId="1" r:id="rId1"/>
@@ -490,7 +490,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -575,11 +575,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -595,33 +610,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="6" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -635,6 +625,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="11" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="11" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -898,20 +915,20 @@
   </sheetPr>
   <dimension ref="A2:P61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.90625" customWidth="1"/>
-    <col min="3" max="3" width="48.6328125" customWidth="1"/>
-    <col min="5" max="5" width="13.90625" customWidth="1"/>
-    <col min="7" max="7" width="53.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.08984375" customWidth="1"/>
-    <col min="11" max="11" width="35.453125" customWidth="1"/>
-    <col min="12" max="12" width="26.90625" customWidth="1"/>
-    <col min="16" max="16" width="17.453125" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" customWidth="1"/>
+    <col min="3" max="3" width="48.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" customWidth="1"/>
+    <col min="7" max="7" width="53.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.109375" customWidth="1"/>
+    <col min="11" max="11" width="35.44140625" customWidth="1"/>
+    <col min="12" max="12" width="26.88671875" customWidth="1"/>
+    <col min="16" max="16" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -953,7 +970,7 @@
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>141.19999999999999</v>
+        <v>142.69999999999999</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="4" t="s">
@@ -965,29 +982,29 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="27"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="16"/>
       <c r="J4" s="5" t="s">
         <v>10</v>
       </c>
       <c r="K4" s="2">
         <f>F7+F13+F20+F43+F45+F46</f>
-        <v>22</v>
+        <v>23.5</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="28"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="30"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="19"/>
       <c r="J5" s="6" t="s">
         <v>11</v>
       </c>
@@ -1111,11 +1128,11 @@
         <v>3</v>
       </c>
       <c r="G10" s="7"/>
-      <c r="J10" s="31" t="s">
+      <c r="J10" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
@@ -1269,7 +1286,7 @@
       </c>
       <c r="G19" s="7"/>
     </row>
-    <row r="20" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>10</v>
       </c>
@@ -1283,11 +1300,11 @@
         <v>5</v>
       </c>
       <c r="F20" s="1">
-        <v>15</v>
+        <v>16.5</v>
       </c>
       <c r="G20" s="12"/>
     </row>
-    <row r="21" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>8</v>
       </c>
@@ -1305,7 +1322,7 @@
       </c>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>8</v>
       </c>
@@ -1323,7 +1340,7 @@
       </c>
       <c r="G22" s="12"/>
     </row>
-    <row r="23" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
         <v>16</v>
       </c>
@@ -1339,7 +1356,7 @@
       </c>
       <c r="G23" s="12"/>
     </row>
-    <row r="24" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>11</v>
       </c>
@@ -1357,7 +1374,7 @@
       </c>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
         <v>16</v>
       </c>
@@ -1373,7 +1390,7 @@
       </c>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
         <v>11</v>
       </c>
@@ -1391,7 +1408,7 @@
       </c>
       <c r="G26" s="12"/>
     </row>
-    <row r="27" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
         <v>16</v>
       </c>
@@ -1407,7 +1424,7 @@
       </c>
       <c r="G27" s="12"/>
     </row>
-    <row r="28" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>11</v>
       </c>
@@ -1425,7 +1442,7 @@
       </c>
       <c r="G28" s="7"/>
     </row>
-    <row r="29" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
         <v>16</v>
       </c>
@@ -1441,7 +1458,7 @@
       </c>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
         <v>11</v>
       </c>
@@ -1459,7 +1476,7 @@
       </c>
       <c r="G30" s="12"/>
     </row>
-    <row r="31" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
         <v>16</v>
       </c>
@@ -1476,7 +1493,7 @@
       <c r="G31" s="12"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="s">
         <v>14</v>
       </c>
@@ -1494,7 +1511,7 @@
       </c>
       <c r="G32" s="7"/>
     </row>
-    <row r="33" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B33" s="8" t="s">
         <v>14</v>
       </c>
@@ -1508,7 +1525,7 @@
       <c r="F33" s="1"/>
       <c r="G33" s="12"/>
     </row>
-    <row r="34" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
         <v>14</v>
       </c>
@@ -1526,7 +1543,7 @@
       </c>
       <c r="G34" s="12"/>
     </row>
-    <row r="35" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
         <v>14</v>
       </c>
@@ -1544,7 +1561,7 @@
       </c>
       <c r="G35" s="12"/>
     </row>
-    <row r="36" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B36" s="8" t="s">
         <v>14</v>
       </c>
@@ -1562,7 +1579,7 @@
       </c>
       <c r="G36" s="12"/>
     </row>
-    <row r="37" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
         <v>14</v>
       </c>
@@ -1580,7 +1597,7 @@
       </c>
       <c r="G37" s="7"/>
     </row>
-    <row r="38" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B38" s="8" t="s">
         <v>14</v>
       </c>
@@ -1598,7 +1615,7 @@
       </c>
       <c r="G38" s="12"/>
     </row>
-    <row r="39" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B39" s="9" t="s">
         <v>15</v>
       </c>
@@ -1616,7 +1633,7 @@
       </c>
       <c r="G39" s="12"/>
     </row>
-    <row r="40" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B40" s="9" t="s">
         <v>15</v>
       </c>
@@ -1634,25 +1651,25 @@
       </c>
       <c r="G40" s="12"/>
     </row>
-    <row r="41" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B41" s="25" t="s">
+    <row r="41" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B41" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="26"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26"/>
-      <c r="G41" s="27"/>
-    </row>
-    <row r="42" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B42" s="28"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="29"/>
-      <c r="F42" s="29"/>
-      <c r="G42" s="30"/>
-    </row>
-    <row r="43" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="16"/>
+    </row>
+    <row r="42" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B42" s="17"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="19"/>
+    </row>
+    <row r="43" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>10</v>
       </c>
@@ -1666,7 +1683,7 @@
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
     </row>
-    <row r="44" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
         <v>11</v>
       </c>
@@ -1680,7 +1697,7 @@
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
         <v>10</v>
       </c>
@@ -1698,7 +1715,7 @@
       </c>
       <c r="G45" s="7"/>
     </row>
-    <row r="46" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
         <v>10</v>
       </c>
@@ -1714,7 +1731,7 @@
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
     </row>
-    <row r="47" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B47" s="8" t="s">
         <v>14</v>
       </c>
@@ -1730,7 +1747,7 @@
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B48" s="9" t="s">
         <v>15</v>
       </c>
@@ -1746,7 +1763,7 @@
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
     </row>
-    <row r="49" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B49" s="9" t="s">
         <v>15</v>
       </c>
@@ -1762,7 +1779,7 @@
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
     </row>
-    <row r="50" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B50" s="9" t="s">
         <v>15</v>
       </c>
@@ -1776,7 +1793,7 @@
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
     </row>
-    <row r="51" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B51" s="9" t="s">
         <v>15</v>
       </c>
@@ -1794,7 +1811,7 @@
       </c>
       <c r="G51" s="7"/>
     </row>
-    <row r="52" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
         <v>8</v>
       </c>
@@ -1812,7 +1829,7 @@
       </c>
       <c r="G52" s="7"/>
     </row>
-    <row r="53" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
         <v>8</v>
       </c>
@@ -1832,7 +1849,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="54" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
         <v>8</v>
       </c>
@@ -1848,7 +1865,7 @@
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
     </row>
-    <row r="55" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B55" s="6" t="s">
         <v>11</v>
       </c>
@@ -1864,7 +1881,7 @@
       </c>
       <c r="G55" s="12"/>
     </row>
-    <row r="56" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B56" s="6" t="s">
         <v>11</v>
       </c>
@@ -1880,7 +1897,7 @@
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
     </row>
-    <row r="57" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B57" s="10" t="s">
         <v>16</v>
       </c>
@@ -1896,7 +1913,7 @@
       </c>
       <c r="G57" s="1"/>
     </row>
-    <row r="58" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B58" s="10" t="s">
         <v>16</v>
       </c>
@@ -1910,7 +1927,7 @@
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
     </row>
-    <row r="59" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B59" s="10" t="s">
         <v>16</v>
       </c>
@@ -1924,7 +1941,7 @@
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
     </row>
-    <row r="60" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B60" s="10" t="s">
         <v>16</v>
       </c>
@@ -1940,7 +1957,7 @@
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
     </row>
-    <row r="61" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B61" s="6" t="s">
         <v>11</v>
       </c>
@@ -1974,41 +1991,43 @@
   </sheetPr>
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6328125" customWidth="1"/>
-    <col min="2" max="2" width="35.453125" customWidth="1"/>
-    <col min="3" max="3" width="27.26953125" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" customWidth="1"/>
-    <col min="7" max="7" width="17.453125" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="35.44140625" customWidth="1"/>
+    <col min="3" max="3" width="27.21875" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="13" t="s">
         <v>63</v>
       </c>
       <c r="K1" s="2">
@@ -2017,741 +2036,808 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
+      <c r="A2" s="22">
         <v>1</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="24">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="23">
         <v>1.5</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="G2" s="16">
+      <c r="G2" s="25">
         <v>45202</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="13" t="s">
         <v>67</v>
       </c>
       <c r="K2" s="2">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="14" x14ac:dyDescent="0.3">
-      <c r="A3" s="13">
+    <row r="3" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A3" s="22">
         <v>2</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="23">
         <v>1.5</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="28">
         <v>45202</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="14" x14ac:dyDescent="0.3">
-      <c r="A4" s="13">
+    <row r="4" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A4" s="22">
         <v>3</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="24">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="23">
         <v>5</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="28">
         <v>45202</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
+      <c r="A5" s="22">
         <v>4</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="26"/>
+      <c r="C5" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="G5" s="11"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="22"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13">
+      <c r="A6" s="22">
         <v>5</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="30"/>
+      <c r="C6" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="23">
         <v>40</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="31">
         <v>45216</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
+      <c r="A7" s="22">
         <v>6</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="32"/>
+      <c r="C7" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="23">
         <v>5</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="G7" s="21">
+      <c r="G7" s="31">
         <v>45216</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13">
+      <c r="A8" s="22">
         <v>7</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="26"/>
+      <c r="C8" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="G8" s="11"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="22"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13">
+      <c r="A9" s="22">
         <v>8</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="2" t="s">
+      <c r="B9" s="26"/>
+      <c r="C9" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="23">
         <v>1.5</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="G9" s="21">
+      <c r="G9" s="31">
         <v>45216</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13">
+      <c r="A10" s="22">
         <v>9</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="2" t="s">
+      <c r="B10" s="26"/>
+      <c r="C10" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="G10" s="11"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="22"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13">
+      <c r="A11" s="22">
         <v>10</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="2" t="s">
+      <c r="B11" s="26"/>
+      <c r="C11" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="G11" s="11"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="22"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13">
+      <c r="A12" s="22">
         <v>11</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="2" t="s">
+      <c r="B12" s="26"/>
+      <c r="C12" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="G12" s="11"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="22"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13">
+      <c r="A13" s="22">
         <v>12</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="2" t="s">
+      <c r="B13" s="26"/>
+      <c r="C13" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="G13" s="11"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="22"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13">
+      <c r="A14" s="22">
         <v>13</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="2" t="s">
+      <c r="B14" s="26"/>
+      <c r="C14" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="G14" s="11"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="22"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13">
+      <c r="A15" s="22">
         <v>14</v>
       </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="2" t="s">
+      <c r="B15" s="26"/>
+      <c r="C15" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="G15" s="11"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="22"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13">
+      <c r="A16" s="22">
         <v>15</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="2" t="s">
+      <c r="B16" s="26"/>
+      <c r="C16" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="G16" s="11"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="22"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13">
+      <c r="A17" s="22">
         <v>16</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="2" t="s">
+      <c r="B17" s="26"/>
+      <c r="C17" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="G17" s="11"/>
-    </row>
-    <row r="18" spans="1:7" ht="14" x14ac:dyDescent="0.3">
-      <c r="A18" s="13">
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="22"/>
+    </row>
+    <row r="18" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A18" s="22">
         <v>17</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="2" t="s">
+      <c r="B18" s="26"/>
+      <c r="C18" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="23">
         <v>3</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="18" t="s">
+      <c r="F18" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="G18" s="21">
+      <c r="G18" s="31">
         <v>45216</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="14" x14ac:dyDescent="0.3">
-      <c r="A19" s="13">
+    <row r="19" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A19" s="22">
         <v>18</v>
       </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="2" t="s">
+      <c r="B19" s="26"/>
+      <c r="C19" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="23">
         <v>3</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="F19" s="18" t="s">
+      <c r="F19" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="G19" s="21">
+      <c r="G19" s="31">
         <v>45216</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="13">
+    <row r="20" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A20" s="22">
         <v>19</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="2" t="s">
+      <c r="B20" s="26"/>
+      <c r="C20" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="G20" s="11"/>
-    </row>
-    <row r="21" spans="1:7" ht="14" x14ac:dyDescent="0.3">
-      <c r="A21" s="13">
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="22"/>
+    </row>
+    <row r="21" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A21" s="22">
         <v>20</v>
       </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="2" t="s">
+      <c r="B21" s="26"/>
+      <c r="C21" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="23">
         <v>2</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="F21" s="18" t="s">
+      <c r="F21" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="G21" s="21">
+      <c r="G21" s="31">
         <v>45216</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="13">
+    <row r="22" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A22" s="22">
         <v>21</v>
       </c>
-      <c r="B22" s="17"/>
-      <c r="C22" s="2" t="s">
+      <c r="B22" s="26"/>
+      <c r="C22" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="G22" s="11"/>
-    </row>
-    <row r="23" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="13">
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="22"/>
+    </row>
+    <row r="23" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A23" s="22">
         <v>22</v>
       </c>
-      <c r="B23" s="17"/>
-      <c r="C23" s="2" t="s">
+      <c r="B23" s="26"/>
+      <c r="C23" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="G23" s="11"/>
-    </row>
-    <row r="24" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="13">
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="22"/>
+    </row>
+    <row r="24" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A24" s="22">
         <v>23</v>
       </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="2" t="s">
+      <c r="B24" s="26"/>
+      <c r="C24" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="23">
         <v>8</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="G24" s="21">
+      <c r="G24" s="31">
         <v>45216</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="13">
+    <row r="25" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A25" s="22">
         <v>24</v>
       </c>
-      <c r="B25" s="17"/>
-      <c r="C25" s="2" t="s">
+      <c r="B25" s="26"/>
+      <c r="C25" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="G25" s="11"/>
-    </row>
-    <row r="26" spans="1:7" ht="14" x14ac:dyDescent="0.3">
-      <c r="A26" s="13">
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="22"/>
+    </row>
+    <row r="26" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A26" s="22">
         <v>25</v>
       </c>
-      <c r="B26" s="17"/>
-      <c r="C26" s="2" t="s">
+      <c r="B26" s="26"/>
+      <c r="C26" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="23">
         <v>5</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="F26" s="18" t="s">
+      <c r="F26" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="G26" s="21">
+      <c r="G26" s="31">
         <v>45216</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="13">
+    <row r="27" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A27" s="22">
         <v>26</v>
       </c>
-      <c r="B27" s="17"/>
-      <c r="C27" s="2" t="s">
+      <c r="B27" s="26"/>
+      <c r="C27" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="G27" s="11"/>
-    </row>
-    <row r="28" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="13">
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="22"/>
+    </row>
+    <row r="28" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A28" s="22">
         <v>27</v>
       </c>
-      <c r="B28" s="15">
+      <c r="B28" s="24">
         <v>1</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="23">
         <v>3</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="G28" s="19">
+      <c r="G28" s="28">
         <v>45202</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="13">
+    <row r="29" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A29" s="22">
         <v>28</v>
       </c>
-      <c r="B29" s="17"/>
-      <c r="C29" s="2" t="s">
+      <c r="B29" s="26"/>
+      <c r="C29" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="G29" s="11"/>
-    </row>
-    <row r="30" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="13">
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="22"/>
+    </row>
+    <row r="30" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A30" s="22">
         <v>29</v>
       </c>
-      <c r="B30" s="17"/>
-      <c r="C30" s="2" t="s">
+      <c r="B30" s="26"/>
+      <c r="C30" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="G30" s="11"/>
-    </row>
-    <row r="31" spans="1:7" ht="14" x14ac:dyDescent="0.3">
-      <c r="A31" s="13">
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="22"/>
+    </row>
+    <row r="31" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A31" s="22">
         <v>30</v>
       </c>
-      <c r="B31" s="15">
+      <c r="B31" s="24">
         <v>1</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="23">
         <v>1</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="E31" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="18" t="s">
+      <c r="F31" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="G31" s="19">
+      <c r="G31" s="28">
         <v>45202</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="14" x14ac:dyDescent="0.3">
-      <c r="A32" s="13">
+    <row r="32" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A32" s="22">
         <v>31</v>
       </c>
-      <c r="B32" s="17"/>
-      <c r="C32" s="2" t="s">
+      <c r="B32" s="26"/>
+      <c r="C32" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="23">
         <v>7</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E32" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="F32" s="18" t="s">
+      <c r="F32" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="G32" s="21">
+      <c r="G32" s="31">
         <v>45216</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="14" x14ac:dyDescent="0.3">
-      <c r="A33" s="13">
+    <row r="33" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A33" s="22">
         <v>32</v>
       </c>
-      <c r="B33" s="22"/>
-      <c r="C33" s="2" t="s">
+      <c r="B33" s="32"/>
+      <c r="C33" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="23">
         <v>0.5</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E33" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="F33" s="18" t="s">
+      <c r="F33" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="G33" s="21">
+      <c r="G33" s="31">
         <v>45216</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="14" x14ac:dyDescent="0.3">
-      <c r="A34" s="13">
+    <row r="34" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A34" s="22">
         <v>33</v>
       </c>
-      <c r="B34" s="17"/>
-      <c r="C34" s="2" t="s">
+      <c r="B34" s="26"/>
+      <c r="C34" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34" s="23">
         <v>1.5</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E34" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="F34" s="18" t="s">
+      <c r="F34" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="G34" s="21">
+      <c r="G34" s="31">
         <v>45216</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="13">
+    <row r="35" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A35" s="22">
         <v>34</v>
       </c>
-      <c r="B35" s="17"/>
-      <c r="C35" s="2" t="s">
+      <c r="B35" s="26"/>
+      <c r="C35" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="G35" s="11"/>
-    </row>
-    <row r="36" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="13">
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="22"/>
+    </row>
+    <row r="36" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A36" s="22">
         <v>35</v>
       </c>
-      <c r="B36" s="17"/>
-      <c r="C36" s="2" t="s">
+      <c r="B36" s="26"/>
+      <c r="C36" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="G36" s="11"/>
-    </row>
-    <row r="37" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="13">
+      <c r="D36" s="29"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="29"/>
+      <c r="G36" s="22"/>
+    </row>
+    <row r="37" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A37" s="22">
         <v>36</v>
       </c>
-      <c r="B37" s="17"/>
-      <c r="C37" s="2" t="s">
+      <c r="B37" s="26"/>
+      <c r="C37" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D37" s="23">
         <v>1</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="E37" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="F37" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="G37" s="23">
+      <c r="G37" s="33">
         <v>45216</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="13">
+    <row r="38" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A38" s="22">
         <v>37</v>
       </c>
-      <c r="B38" s="17"/>
-      <c r="C38" s="2" t="s">
+      <c r="B38" s="26"/>
+      <c r="C38" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="G38" s="11"/>
-    </row>
-    <row r="39" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="13">
+      <c r="D38" s="29"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="22"/>
+    </row>
+    <row r="39" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A39" s="22">
         <v>38</v>
       </c>
-      <c r="B39" s="17"/>
-      <c r="C39" s="2" t="s">
+      <c r="B39" s="26"/>
+      <c r="C39" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="G39" s="11"/>
-    </row>
-    <row r="40" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="13">
+      <c r="D39" s="29"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="22"/>
+    </row>
+    <row r="40" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A40" s="22">
         <v>39</v>
       </c>
-      <c r="B40" s="17"/>
-      <c r="C40" s="2" t="s">
+      <c r="B40" s="26"/>
+      <c r="C40" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D40" s="23">
         <v>3</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="E40" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F40" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="G40" s="21">
+      <c r="G40" s="31">
         <v>45216</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="13">
+    <row r="41" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A41" s="22">
         <v>40</v>
       </c>
-      <c r="B41" s="17"/>
-      <c r="C41" s="2" t="s">
+      <c r="B41" s="26"/>
+      <c r="C41" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D41" s="23">
         <v>2</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="E41" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="F41" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="G41" s="21">
+      <c r="G41" s="31">
         <v>45216</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A42" s="13">
+    <row r="42" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A42" s="22">
         <v>41</v>
       </c>
-      <c r="B42" s="17"/>
-      <c r="C42" s="2" t="s">
+      <c r="B42" s="26"/>
+      <c r="C42" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D42" s="23">
         <v>2</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="E42" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="F42" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="G42" s="21">
+      <c r="G42" s="31">
         <v>45216</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="13">
+    <row r="43" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A43" s="22">
         <v>42</v>
       </c>
-      <c r="B43" s="17"/>
-      <c r="C43" s="2" t="s">
+      <c r="B43" s="26"/>
+      <c r="C43" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D43" s="23">
         <v>3</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="E43" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="F43" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="G43" s="21">
+      <c r="G43" s="31">
         <v>45216</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="14" x14ac:dyDescent="0.3">
-      <c r="A44" s="13">
+    <row r="44" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A44" s="22">
         <v>43</v>
       </c>
-      <c r="B44" s="15">
+      <c r="B44" s="24">
         <v>1</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D44" s="23">
         <v>0.5</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="E44" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="F44" s="18" t="s">
+      <c r="F44" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="G44" s="21">
+      <c r="G44" s="31">
         <v>45216</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="13">
+    <row r="45" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A45" s="22">
         <v>44</v>
       </c>
-      <c r="B45" s="22"/>
-      <c r="C45" s="2" t="s">
+      <c r="B45" s="32"/>
+      <c r="C45" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="D45" s="2">
+      <c r="D45" s="23">
         <v>1.5</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="E45" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="F45" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="G45" s="21">
+      <c r="G45" s="31">
         <v>45216</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="13">
+    <row r="46" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A46" s="22">
         <v>45</v>
       </c>
-      <c r="B46" s="17"/>
-      <c r="C46" s="2" t="s">
+      <c r="B46" s="26"/>
+      <c r="C46" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="G46" s="11"/>
-    </row>
-    <row r="47" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
+      <c r="D46" s="29"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="29"/>
+      <c r="G46" s="22"/>
+    </row>
+    <row r="47" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A47" s="22">
         <v>46</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="B47" s="29"/>
+      <c r="C47" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="D47" s="2">
+      <c r="D47" s="23">
         <v>2</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="E47" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="F47" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="G47" s="24">
+      <c r="G47" s="34">
         <v>45216</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Camara 1.1 (Foto en BBDD)
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 1ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 1ª Version.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34616\Desktop\CEU\tercer año\ing_software\Konguitos_Casino\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanzc\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78ED14EC-C1B9-4839-A6FA-D199B53E3428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E61E99F-998F-4155-AC2B-41A6CAF144F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificador" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="113">
   <si>
     <t>Nombre</t>
   </si>
@@ -369,6 +369,12 @@
   </si>
   <si>
     <t>Animación tragaperras</t>
+  </si>
+  <si>
+    <t>Interfaz Funciones Admin</t>
+  </si>
+  <si>
+    <t>Poner la foto en la BBDD</t>
   </si>
 </sst>
 </file>
@@ -916,22 +922,22 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:P62"/>
+  <dimension ref="A2:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" customWidth="1"/>
-    <col min="3" max="3" width="48.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" customWidth="1"/>
-    <col min="7" max="7" width="53.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.109375" customWidth="1"/>
-    <col min="11" max="11" width="35.44140625" customWidth="1"/>
-    <col min="12" max="12" width="26.88671875" customWidth="1"/>
-    <col min="16" max="16" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.90625" customWidth="1"/>
+    <col min="3" max="3" width="48.6328125" customWidth="1"/>
+    <col min="5" max="5" width="13.90625" customWidth="1"/>
+    <col min="7" max="7" width="53.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.08984375" customWidth="1"/>
+    <col min="11" max="11" width="35.453125" customWidth="1"/>
+    <col min="12" max="12" width="26.90625" customWidth="1"/>
+    <col min="16" max="16" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -968,19 +974,19 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:F3" si="0">SUM(E6:E1004)</f>
+        <f t="shared" ref="E3:F3" si="0">SUM(E6:E1006)</f>
         <v>112.5</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>155.29999999999998</v>
+        <v>158.29999999999998</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="K3" s="2">
-        <f>F6+F12+F22+F21+F52+F53+F54+F62</f>
+        <f>F6+F12+F22+F21+F54+F55+F56+F64</f>
         <v>45</v>
       </c>
     </row>
@@ -1012,7 +1018,7 @@
         <v>11</v>
       </c>
       <c r="K5" s="2">
-        <f>F8+F14+F19+F24+F26+F28+F30+F44+F55+F56+F61</f>
+        <f>F8+F14+F19+F24+F26+F28+F30+F44+F57+F58+F63</f>
         <v>33.350000000000009</v>
       </c>
       <c r="L5" s="2"/>
@@ -1038,7 +1044,7 @@
         <v>14</v>
       </c>
       <c r="K6" s="2">
-        <f>F9+F15+F32+F33+F34+F35+F36+F37+F38+F47</f>
+        <f>F9+F15+F32+F33+F34+F35+F36+F37+F38+F49</f>
         <v>29.6</v>
       </c>
       <c r="L6" s="2"/>
@@ -1064,7 +1070,7 @@
         <v>15</v>
       </c>
       <c r="K7" s="2">
-        <f>F10+F16+F39+F40+F48+F49+F50+F51</f>
+        <f>F10+F16+F39+F40+F50+F51+F52+F53</f>
         <v>16</v>
       </c>
       <c r="L7" s="2"/>
@@ -1090,7 +1096,7 @@
         <v>16</v>
       </c>
       <c r="K8" s="2">
-        <f>F11+F23+F25+F27+F29+F31+F57+F58+F59+F60</f>
+        <f>F11+F23+F25+F27+F29+F31+F59+F60+F61+F62</f>
         <v>5.35</v>
       </c>
       <c r="L8" s="2"/>
@@ -1289,7 +1295,7 @@
       </c>
       <c r="G19" s="7"/>
     </row>
-    <row r="20" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>10</v>
       </c>
@@ -1307,7 +1313,7 @@
       </c>
       <c r="G20" s="12"/>
     </row>
-    <row r="21" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>8</v>
       </c>
@@ -1325,7 +1331,7 @@
       </c>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>8</v>
       </c>
@@ -1343,7 +1349,7 @@
       </c>
       <c r="G22" s="12"/>
     </row>
-    <row r="23" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
         <v>16</v>
       </c>
@@ -1359,7 +1365,7 @@
       </c>
       <c r="G23" s="12"/>
     </row>
-    <row r="24" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>11</v>
       </c>
@@ -1377,7 +1383,7 @@
       </c>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
         <v>16</v>
       </c>
@@ -1393,7 +1399,7 @@
       </c>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
         <v>11</v>
       </c>
@@ -1411,7 +1417,7 @@
       </c>
       <c r="G26" s="12"/>
     </row>
-    <row r="27" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
         <v>16</v>
       </c>
@@ -1427,7 +1433,7 @@
       </c>
       <c r="G27" s="12"/>
     </row>
-    <row r="28" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>11</v>
       </c>
@@ -1445,7 +1451,7 @@
       </c>
       <c r="G28" s="7"/>
     </row>
-    <row r="29" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
         <v>16</v>
       </c>
@@ -1461,7 +1467,7 @@
       </c>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
         <v>11</v>
       </c>
@@ -1479,7 +1485,7 @@
       </c>
       <c r="G30" s="12"/>
     </row>
-    <row r="31" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
         <v>16</v>
       </c>
@@ -1496,7 +1502,7 @@
       <c r="G31" s="12"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="2:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="s">
         <v>14</v>
       </c>
@@ -1514,7 +1520,7 @@
       </c>
       <c r="G32" s="7"/>
     </row>
-    <row r="33" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B33" s="8" t="s">
         <v>14</v>
       </c>
@@ -1528,7 +1534,7 @@
       <c r="F33" s="1"/>
       <c r="G33" s="12"/>
     </row>
-    <row r="34" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
         <v>14</v>
       </c>
@@ -1546,7 +1552,7 @@
       </c>
       <c r="G34" s="12"/>
     </row>
-    <row r="35" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
         <v>14</v>
       </c>
@@ -1564,7 +1570,7 @@
       </c>
       <c r="G35" s="12"/>
     </row>
-    <row r="36" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B36" s="8" t="s">
         <v>14</v>
       </c>
@@ -1582,7 +1588,7 @@
       </c>
       <c r="G36" s="12"/>
     </row>
-    <row r="37" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
         <v>14</v>
       </c>
@@ -1600,7 +1606,7 @@
       </c>
       <c r="G37" s="7"/>
     </row>
-    <row r="38" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B38" s="8" t="s">
         <v>14</v>
       </c>
@@ -1618,7 +1624,7 @@
       </c>
       <c r="G38" s="12"/>
     </row>
-    <row r="39" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B39" s="9" t="s">
         <v>15</v>
       </c>
@@ -1636,7 +1642,7 @@
       </c>
       <c r="G39" s="12"/>
     </row>
-    <row r="40" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B40" s="9" t="s">
         <v>15</v>
       </c>
@@ -1654,7 +1660,7 @@
       </c>
       <c r="G40" s="12"/>
     </row>
-    <row r="41" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B41" s="27" t="s">
         <v>36</v>
       </c>
@@ -1664,7 +1670,7 @@
       <c r="F41" s="28"/>
       <c r="G41" s="29"/>
     </row>
-    <row r="42" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B42" s="30"/>
       <c r="C42" s="31"/>
       <c r="D42" s="31"/>
@@ -1672,7 +1678,7 @@
       <c r="F42" s="31"/>
       <c r="G42" s="32"/>
     </row>
-    <row r="43" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>10</v>
       </c>
@@ -1686,7 +1692,7 @@
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
     </row>
-    <row r="44" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
         <v>11</v>
       </c>
@@ -1700,7 +1706,7 @@
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
         <v>10</v>
       </c>
@@ -1718,7 +1724,7 @@
       </c>
       <c r="G45" s="7"/>
     </row>
-    <row r="46" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
         <v>10</v>
       </c>
@@ -1734,265 +1740,293 @@
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
     </row>
-    <row r="47" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B47" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>40</v>
+        <v>112</v>
       </c>
       <c r="D47" s="1">
-        <v>23</v>
-      </c>
-      <c r="E47" s="1">
-        <v>8</v>
-      </c>
-      <c r="F47" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1">
+        <v>3</v>
+      </c>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B48" s="9" t="s">
-        <v>15</v>
+    <row r="48" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B48" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E48" s="1">
-        <v>3</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
     </row>
-    <row r="49" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B49" s="9" t="s">
-        <v>15</v>
+    <row r="49" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B49" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D49" s="1">
+        <v>23</v>
+      </c>
+      <c r="E49" s="1">
         <v>8</v>
-      </c>
-      <c r="E49" s="1">
-        <v>1.5</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
     </row>
-    <row r="50" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B50" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E50" s="1"/>
+      <c r="E50" s="1">
+        <v>3</v>
+      </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
     </row>
-    <row r="51" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B51" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D51" s="1">
+        <v>8</v>
+      </c>
+      <c r="E51" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+    </row>
+    <row r="52" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B52" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="E51" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="F51" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="G51" s="7"/>
-    </row>
-    <row r="52" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B52" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E52" s="1">
-        <v>0</v>
-      </c>
-      <c r="F52" s="1">
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+    </row>
+    <row r="53" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B53" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D53" s="1">
+        <v>43</v>
+      </c>
+      <c r="E53" s="1">
         <v>0.5</v>
       </c>
-      <c r="G52" s="7"/>
-    </row>
-    <row r="53" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B53" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D53" s="1">
-        <v>36</v>
-      </c>
-      <c r="E53" s="1">
-        <v>1</v>
-      </c>
       <c r="F53" s="1">
-        <v>1</v>
-      </c>
-      <c r="G53" s="12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="54" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+      <c r="G53" s="7"/>
+    </row>
+    <row r="54" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E54" s="1">
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G54" s="7"/>
+    </row>
+    <row r="55" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D55" s="1">
+        <v>36</v>
+      </c>
+      <c r="E55" s="1">
+        <v>1</v>
+      </c>
+      <c r="F55" s="1">
+        <v>1</v>
+      </c>
+      <c r="G55" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D54" s="1">
+      <c r="D56" s="1">
         <v>5</v>
       </c>
-      <c r="E54" s="1">
+      <c r="E56" s="1">
         <v>40</v>
-      </c>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-    </row>
-    <row r="55" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B55" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1">
-        <v>3</v>
-      </c>
-      <c r="F55" s="1">
-        <v>5.5</v>
-      </c>
-      <c r="G55" s="12"/>
-    </row>
-    <row r="56" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B56" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D56" s="1">
-        <v>39</v>
-      </c>
-      <c r="E56" s="1">
-        <v>3</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
     </row>
-    <row r="57" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B57" s="10" t="s">
-        <v>16</v>
+    <row r="57" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B57" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E57" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1">
+        <v>3</v>
+      </c>
       <c r="F57" s="1">
-        <v>1</v>
-      </c>
-      <c r="G57" s="1"/>
-    </row>
-    <row r="58" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B58" s="10" t="s">
-        <v>16</v>
+        <v>5.5</v>
+      </c>
+      <c r="G57" s="12"/>
+    </row>
+    <row r="58" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B58" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E58" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="D58" s="1">
+        <v>39</v>
+      </c>
+      <c r="E58" s="1">
+        <v>3</v>
+      </c>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
     </row>
-    <row r="59" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B59" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D59" s="1">
-        <v>41</v>
+        <v>51</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
+      <c r="F59" s="1">
+        <v>1</v>
+      </c>
       <c r="G59" s="1"/>
     </row>
-    <row r="60" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B60" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E60" s="1">
-        <v>2</v>
-      </c>
+      <c r="E60" s="1"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
     </row>
-    <row r="61" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B61" s="6" t="s">
-        <v>11</v>
+    <row r="61" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B61" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="F61" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="G61" s="12"/>
-    </row>
-    <row r="62" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="4" t="s">
-        <v>8</v>
+        <v>53</v>
+      </c>
+      <c r="D61" s="1">
+        <v>41</v>
+      </c>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+    </row>
+    <row r="62" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B62" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>110</v>
+        <v>54</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E62" s="1">
+        <v>2</v>
+      </c>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+    </row>
+    <row r="63" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B63" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F63" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="G63" s="12"/>
+    </row>
+    <row r="64" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E64" s="1">
         <v>0</v>
       </c>
-      <c r="F62" s="1">
+      <c r="F64" s="1">
         <v>0.5</v>
       </c>
-      <c r="G62" s="7"/>
+      <c r="G64" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2016,13 +2050,13 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="35.44140625" customWidth="1"/>
-    <col min="3" max="3" width="27.21875" customWidth="1"/>
-    <col min="4" max="4" width="10.21875" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="14.6328125" customWidth="1"/>
+    <col min="2" max="2" width="35.453125" customWidth="1"/>
+    <col min="3" max="3" width="27.1796875" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" customWidth="1"/>
+    <col min="7" max="7" width="17.453125" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2085,7 +2119,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="14">
         <v>2</v>
       </c>
@@ -2106,7 +2140,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="14">
         <v>3</v>
       </c>
@@ -2322,7 +2356,7 @@
       <c r="F17" s="21"/>
       <c r="G17" s="14"/>
     </row>
-    <row r="18" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A18" s="14">
         <v>17</v>
       </c>
@@ -2343,7 +2377,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A19" s="14">
         <v>18</v>
       </c>
@@ -2364,7 +2398,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A20" s="14">
         <v>19</v>
       </c>
@@ -2377,7 +2411,7 @@
       <c r="F20" s="21"/>
       <c r="G20" s="14"/>
     </row>
-    <row r="21" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A21" s="14">
         <v>20</v>
       </c>
@@ -2398,7 +2432,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A22" s="14">
         <v>21</v>
       </c>
@@ -2411,7 +2445,7 @@
       <c r="F22" s="21"/>
       <c r="G22" s="14"/>
     </row>
-    <row r="23" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A23" s="14">
         <v>22</v>
       </c>
@@ -2424,7 +2458,7 @@
       <c r="F23" s="21"/>
       <c r="G23" s="14"/>
     </row>
-    <row r="24" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A24" s="14">
         <v>23</v>
       </c>
@@ -2445,7 +2479,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A25" s="14">
         <v>24</v>
       </c>
@@ -2458,7 +2492,7 @@
       <c r="F25" s="21"/>
       <c r="G25" s="14"/>
     </row>
-    <row r="26" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A26" s="14">
         <v>25</v>
       </c>
@@ -2479,7 +2513,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A27" s="14">
         <v>26</v>
       </c>
@@ -2492,7 +2526,7 @@
       <c r="F27" s="21"/>
       <c r="G27" s="14"/>
     </row>
-    <row r="28" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A28" s="14">
         <v>27</v>
       </c>
@@ -2515,7 +2549,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A29" s="14">
         <v>28</v>
       </c>
@@ -2528,7 +2562,7 @@
       <c r="F29" s="21"/>
       <c r="G29" s="14"/>
     </row>
-    <row r="30" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A30" s="14">
         <v>29</v>
       </c>
@@ -2541,7 +2575,7 @@
       <c r="F30" s="21"/>
       <c r="G30" s="14"/>
     </row>
-    <row r="31" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A31" s="14">
         <v>30</v>
       </c>
@@ -2564,7 +2598,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A32" s="14">
         <v>31</v>
       </c>
@@ -2585,7 +2619,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A33" s="14">
         <v>32</v>
       </c>
@@ -2606,7 +2640,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A34" s="14">
         <v>33</v>
       </c>
@@ -2627,7 +2661,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A35" s="14">
         <v>34</v>
       </c>
@@ -2640,7 +2674,7 @@
       <c r="F35" s="21"/>
       <c r="G35" s="14"/>
     </row>
-    <row r="36" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A36" s="14">
         <v>35</v>
       </c>
@@ -2653,7 +2687,7 @@
       <c r="F36" s="21"/>
       <c r="G36" s="14"/>
     </row>
-    <row r="37" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A37" s="14">
         <v>36</v>
       </c>
@@ -2674,7 +2708,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A38" s="14">
         <v>37</v>
       </c>
@@ -2687,7 +2721,7 @@
       <c r="F38" s="21"/>
       <c r="G38" s="14"/>
     </row>
-    <row r="39" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A39" s="14">
         <v>38</v>
       </c>
@@ -2700,7 +2734,7 @@
       <c r="F39" s="21"/>
       <c r="G39" s="14"/>
     </row>
-    <row r="40" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A40" s="14">
         <v>39</v>
       </c>
@@ -2721,7 +2755,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A41" s="14">
         <v>40</v>
       </c>
@@ -2742,7 +2776,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A42" s="14">
         <v>41</v>
       </c>
@@ -2763,7 +2797,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A43" s="14">
         <v>42</v>
       </c>
@@ -2784,7 +2818,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A44" s="14">
         <v>43</v>
       </c>
@@ -2807,7 +2841,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A45" s="14">
         <v>44</v>
       </c>
@@ -2828,7 +2862,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A46" s="14">
         <v>45</v>
       </c>
@@ -2841,7 +2875,7 @@
       <c r="F46" s="21"/>
       <c r="G46" s="14"/>
     </row>
-    <row r="47" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A47" s="14">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
toolbar + saldo cartas
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 1ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 1ª Version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34616\Desktop\CEU\tercer año\ing_software\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78ED14EC-C1B9-4839-A6FA-D199B53E3428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4307FD2-1A21-4E8B-A4B8-09110A617F8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -918,8 +918,8 @@
   </sheetPr>
   <dimension ref="A2:P62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -973,7 +973,7 @@
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>155.29999999999998</v>
+        <v>163.66999999999999</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="4" t="s">
@@ -1013,7 +1013,7 @@
       </c>
       <c r="K5" s="2">
         <f>F8+F14+F19+F24+F26+F28+F30+F44+F55+F56+F61</f>
-        <v>33.350000000000009</v>
+        <v>41.720000000000006</v>
       </c>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
@@ -1475,7 +1475,7 @@
         <v>3</v>
       </c>
       <c r="F30" s="1">
-        <v>20.6</v>
+        <v>22.17</v>
       </c>
       <c r="G30" s="12"/>
     </row>
@@ -1697,8 +1697,10 @@
         <v>13</v>
       </c>
       <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
+      <c r="F44" s="1">
+        <v>5.8</v>
+      </c>
+      <c r="G44" s="12"/>
     </row>
     <row r="45" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
@@ -1880,7 +1882,7 @@
         <v>3</v>
       </c>
       <c r="F55" s="1">
-        <v>5.5</v>
+        <v>6.5</v>
       </c>
       <c r="G55" s="12"/>
     </row>

</xml_diff>